<commit_message>
Implemented new functionality:  - block IDs starts at value 2  - added CompiledConfigID parameter in NvM.epc
</commit_message>
<xml_diff>
--- a/MEM_configurator_test_plan.xlsx
+++ b/MEM_configurator_test_plan.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="126">
   <si>
     <t>Requirements</t>
   </si>
@@ -814,9 +814,6 @@
     <t>Check that the resistent blocks are mapped first</t>
   </si>
   <si>
-    <t>- Check that the resistnat block has an higher ID than the other block</t>
-  </si>
-  <si>
     <t>Check the output format of the NvDM file</t>
   </si>
   <si>
@@ -927,6 +924,70 @@
   <si>
     <t>- initial creation 
 - created tests for MEM_configurator</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Check the block IDs</t>
+  </si>
+  <si>
+    <t>- Check that the resistent block has an higher ID than the other block</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Provide two block that are correctly defined to the tool</t>
+    </r>
+  </si>
+  <si>
+    <t>- Check that the identifiers starts with 2, and are consecutive</t>
+  </si>
+  <si>
+    <t>TBD_2</t>
+  </si>
+  <si>
+    <t>Check that the tool admits only one CompiledCheckID</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Provide to the tool one block correctly defined, and one configuration file that has more than one CompiledCheckID parameter defined</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1387,9 +1448,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1402,192 +1478,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2019,7 +1920,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>17</v>
@@ -2129,13 +2030,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="E42" sqref="E42:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2193,10 +2094,10 @@
         <v>24</v>
       </c>
       <c r="B3" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>116</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>117</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>7</v>
@@ -2213,10 +2114,10 @@
         <v>25</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>9</v>
@@ -2233,10 +2134,10 @@
         <v>26</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>9</v>
@@ -2252,7 +2153,7 @@
       <c r="A6" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="45" t="s">
         <v>75</v>
       </c>
       <c r="C6" s="19" t="s">
@@ -2270,7 +2171,7 @@
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="46"/>
-      <c r="B7" s="41"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="19" t="s">
         <v>20</v>
       </c>
@@ -2285,10 +2186,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="49" t="s">
         <v>49</v>
       </c>
       <c r="C8" s="19" t="s">
@@ -2305,8 +2206,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="45"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="19" t="s">
         <v>52</v>
       </c>
@@ -2341,10 +2242,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="49" t="s">
         <v>76</v>
       </c>
       <c r="C11" s="19" t="s">
@@ -2361,8 +2262,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="45"/>
+      <c r="A12" s="48"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="19" t="s">
         <v>78</v>
       </c>
@@ -2377,10 +2278,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="49" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="19" t="s">
@@ -2397,8 +2298,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="48"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="19" t="s">
         <v>79</v>
       </c>
@@ -2413,8 +2314,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
-      <c r="B15" s="45"/>
+      <c r="A15" s="48"/>
+      <c r="B15" s="50"/>
       <c r="C15" s="19" t="s">
         <v>58</v>
       </c>
@@ -2432,7 +2333,7 @@
       <c r="A16" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="45" t="s">
         <v>59</v>
       </c>
       <c r="C16" s="19" t="s">
@@ -2450,7 +2351,7 @@
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="46"/>
-      <c r="B17" s="41"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="19" t="s">
         <v>61</v>
       </c>
@@ -2485,10 +2386,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="49" t="s">
         <v>64</v>
       </c>
       <c r="C19" s="19" t="s">
@@ -2505,8 +2406,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="48"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="19" t="s">
         <v>81</v>
       </c>
@@ -2521,8 +2422,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="48"/>
+      <c r="A21" s="51"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="19" t="s">
         <v>82</v>
       </c>
@@ -2537,8 +2438,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="45"/>
+      <c r="A22" s="48"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="19" t="s">
         <v>83</v>
       </c>
@@ -2553,10 +2454,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="49" t="s">
         <v>67</v>
       </c>
       <c r="C23" s="20" t="s">
@@ -2573,8 +2474,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="45"/>
+      <c r="A24" s="48"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="20" t="s">
         <v>85</v>
       </c>
@@ -2632,7 +2533,7 @@
       <c r="A27" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="45" t="s">
         <v>70</v>
       </c>
       <c r="C27" s="19" t="s">
@@ -2650,7 +2551,7 @@
     </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="46"/>
-      <c r="B28" s="41"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="19" t="s">
         <v>87</v>
       </c>
@@ -2675,7 +2576,7 @@
         <v>69</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>5</v>
@@ -2685,10 +2586,10 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="45" t="s">
         <v>88</v>
       </c>
       <c r="C30" s="19" t="s">
@@ -2705,8 +2606,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
-      <c r="B31" s="41"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="45"/>
       <c r="C31" s="19" t="s">
         <v>87</v>
       </c>
@@ -2761,10 +2662,10 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="49" t="s">
         <v>94</v>
       </c>
       <c r="C34" s="29" t="s">
@@ -2781,8 +2682,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="43"/>
-      <c r="B35" s="45"/>
+      <c r="A35" s="48"/>
+      <c r="B35" s="50"/>
       <c r="C35" s="29" t="s">
         <v>97</v>
       </c>
@@ -2804,7 +2705,7 @@
         <v>99</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D36" s="24" t="s">
         <v>55</v>
@@ -2824,10 +2725,10 @@
         <v>100</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>5</v>
@@ -2837,16 +2738,16 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="52" t="s">
+      <c r="C38" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D38" s="51" t="s">
+      <c r="D38" s="43" t="s">
         <v>9</v>
       </c>
       <c r="E38" s="5" t="s">
@@ -2861,13 +2762,13 @@
         <v>46</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C39" s="19" t="s">
         <v>69</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>5</v>
@@ -2881,13 +2782,13 @@
         <v>47</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C40" s="19" t="s">
         <v>69</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>5</v>
@@ -2897,16 +2798,16 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="52" t="s">
+      <c r="C41" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="D41" s="51" t="s">
+      <c r="D41" s="43" t="s">
         <v>9</v>
       </c>
       <c r="E41" s="5" t="s">
@@ -2916,21 +2817,61 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="35" t="s">
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B44" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="B42" s="40" t="s">
+      <c r="C44" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" s="6" t="s">
+      <c r="D44" s="27"/>
+      <c r="E44" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F44" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2958,7 +2899,7 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
   </mergeCells>
-  <conditionalFormatting sqref="E29:E1048576 E1:E24">
+  <conditionalFormatting sqref="E1:E24 E29:E1048576">
     <cfRule type="cellIs" dxfId="11" priority="31" operator="equal">
       <formula>"done"</formula>
     </cfRule>
@@ -2966,12 +2907,12 @@
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F29:F42 F2:F24">
+  <conditionalFormatting sqref="F2:F24 F29:F44">
     <cfRule type="cellIs" dxfId="9" priority="30" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F29:F42 F2:F24">
+  <conditionalFormatting sqref="F2:F24 F29:F44">
     <cfRule type="cellIs" dxfId="8" priority="29" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
@@ -2995,10 +2936,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E44">
       <formula1>"done, not done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F44">
       <formula1>"YES, NO"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Implemented new functionality:  - non-mandatory parameters are not generated in NvM.epc if input data is not complete
</commit_message>
<xml_diff>
--- a/MEM_configurator_test_plan.xlsx
+++ b/MEM_configurator_test_plan.xlsx
@@ -852,29 +852,6 @@
     <t>- Check that the NvM block has set all the required parameters</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Provide to the tool one block correctly defined, and one profile that doesn't have all the necessary parameters defined</t>
-    </r>
-  </si>
-  <si>
     <t>CHECK.XML</t>
   </si>
   <si>
@@ -987,6 +964,29 @@
         <scheme val="minor"/>
       </rPr>
       <t>: Provide to the tool one block correctly defined, and one configuration file that has more than one CompiledCheckID parameter defined</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Provide to the tool one block correctly defined, and one profile that doesn't have all the necessary mandatory parameters defined</t>
     </r>
   </si>
 </sst>
@@ -1460,75 +1460,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1920,7 +1880,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>17</v>
@@ -2036,7 +1996,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E42" sqref="E42:F43"/>
+      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,10 +2054,10 @@
         <v>24</v>
       </c>
       <c r="B3" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>115</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>116</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>7</v>
@@ -2114,10 +2074,10 @@
         <v>25</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>9</v>
@@ -2134,10 +2094,10 @@
         <v>26</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>9</v>
@@ -2150,10 +2110,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="51" t="s">
         <v>75</v>
       </c>
       <c r="C6" s="19" t="s">
@@ -2170,8 +2130,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="45"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="19" t="s">
         <v>20</v>
       </c>
@@ -2186,10 +2146,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="47" t="s">
         <v>49</v>
       </c>
       <c r="C8" s="19" t="s">
@@ -2206,8 +2166,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="48"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="48"/>
       <c r="C9" s="19" t="s">
         <v>52</v>
       </c>
@@ -2242,10 +2202,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="47" t="s">
         <v>76</v>
       </c>
       <c r="C11" s="19" t="s">
@@ -2262,8 +2222,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="50"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="19" t="s">
         <v>78</v>
       </c>
@@ -2278,10 +2238,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="47" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="19" t="s">
@@ -2298,8 +2258,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
-      <c r="B14" s="52"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="19" t="s">
         <v>79</v>
       </c>
@@ -2314,8 +2274,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
-      <c r="B15" s="50"/>
+      <c r="A15" s="46"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="19" t="s">
         <v>58</v>
       </c>
@@ -2330,10 +2290,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="51" t="s">
         <v>59</v>
       </c>
       <c r="C16" s="19" t="s">
@@ -2350,8 +2310,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
-      <c r="B17" s="45"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="19" t="s">
         <v>61</v>
       </c>
@@ -2386,10 +2346,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="47" t="s">
         <v>64</v>
       </c>
       <c r="C19" s="19" t="s">
@@ -2406,8 +2366,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
-      <c r="B20" s="52"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="19" t="s">
         <v>81</v>
       </c>
@@ -2422,8 +2382,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="52"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="19" t="s">
         <v>82</v>
       </c>
@@ -2438,8 +2398,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
-      <c r="B22" s="50"/>
+      <c r="A22" s="46"/>
+      <c r="B22" s="48"/>
       <c r="C22" s="19" t="s">
         <v>83</v>
       </c>
@@ -2454,10 +2414,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="47" t="s">
         <v>67</v>
       </c>
       <c r="C23" s="20" t="s">
@@ -2474,8 +2434,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
-      <c r="B24" s="50"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="48"/>
       <c r="C24" s="20" t="s">
         <v>85</v>
       </c>
@@ -2530,10 +2490,10 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="51" t="s">
         <v>70</v>
       </c>
       <c r="C27" s="19" t="s">
@@ -2550,8 +2510,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="46"/>
-      <c r="B28" s="45"/>
+      <c r="A28" s="52"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="19" t="s">
         <v>87</v>
       </c>
@@ -2586,10 +2546,10 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="45" t="s">
+      <c r="B30" s="51" t="s">
         <v>88</v>
       </c>
       <c r="C30" s="19" t="s">
@@ -2606,8 +2566,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
-      <c r="B31" s="45"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="19" t="s">
         <v>87</v>
       </c>
@@ -2662,10 +2622,10 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="47" t="s">
+      <c r="A34" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="47" t="s">
         <v>94</v>
       </c>
       <c r="C34" s="29" t="s">
@@ -2682,8 +2642,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="48"/>
-      <c r="B35" s="50"/>
+      <c r="A35" s="46"/>
+      <c r="B35" s="48"/>
       <c r="C35" s="29" t="s">
         <v>97</v>
       </c>
@@ -2705,7 +2665,7 @@
         <v>99</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="D36" s="24" t="s">
         <v>55</v>
@@ -2728,7 +2688,7 @@
         <v>105</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>5</v>
@@ -2819,16 +2779,16 @@
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="42" t="s">
-        <v>119</v>
-      </c>
       <c r="C42" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42" s="43" t="s">
         <v>121</v>
-      </c>
-      <c r="D42" s="43" t="s">
-        <v>122</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>5</v>
@@ -2839,13 +2799,13 @@
     </row>
     <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="B43" s="42" t="s">
+      <c r="C43" s="19" t="s">
         <v>124</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>125</v>
       </c>
       <c r="D43" s="24" t="s">
         <v>55</v>
@@ -2859,13 +2819,13 @@
     </row>
     <row r="44" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B44" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="B44" s="40" t="s">
+      <c r="C44" s="26" t="s">
         <v>109</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>110</v>
       </c>
       <c r="D44" s="27"/>
       <c r="E44" s="5" t="s">
@@ -2878,18 +2838,6 @@
   </sheetData>
   <autoFilter ref="A1:E27"/>
   <mergeCells count="20">
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A27:A28"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A16:A17"/>
@@ -2898,40 +2846,52 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E24 E29:E1048576">
-    <cfRule type="cellIs" dxfId="11" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="31" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="32" operator="equal">
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F24 F29:F44">
-    <cfRule type="cellIs" dxfId="9" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="30" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F24 F29:F44">
-    <cfRule type="cellIs" dxfId="8" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="29" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25:E28">
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="12" operator="equal">
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:F28">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:F28">
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Evolutions:  - ports instead of interfaces defined for each block  - CONSISTENCY and CRC optional for profile definition  - replaced plugin name by "/AUTOSAR/EcuDefs/" in the output files  - modified tests according to mentioned updates
</commit_message>
<xml_diff>
--- a/MEM_configurator_test_plan.xlsx
+++ b/MEM_configurator_test_plan.xlsx
@@ -305,52 +305,6 @@
     <t>Check that the tool will correctly behave when the referenced interfaces are not defined in the input files</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Provide to the tool on block that references three interfaces, and another files which contains the definition of these interfaces</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Provide to the tool on block that references three interfaces, and another files which does not contains the definition of all these interfaces</t>
-    </r>
-  </si>
-  <si>
     <t>Check that the tool will correctly behave when the same interface is referenced multiple times</t>
   </si>
   <si>
@@ -987,6 +941,52 @@
         <scheme val="minor"/>
       </rPr>
       <t>: Provide two blocks that are correctly defined to the tool</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Provide to the tool on block that references three ports, and another file which contains the interfaces referenced by these ports</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Provide to the tool on block that references three ports, and another file which does not contain the interfaces referenced by these ports</t>
     </r>
   </si>
 </sst>
@@ -1460,28 +1460,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1880,7 +1880,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>17</v>
@@ -1993,10 +1993,10 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2054,10 +2054,10 @@
         <v>22</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>7</v>
@@ -2074,10 +2074,10 @@
         <v>23</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>9</v>
@@ -2094,10 +2094,10 @@
         <v>24</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>9</v>
@@ -2110,14 +2110,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="45" t="s">
-        <v>73</v>
+      <c r="B6" s="51" t="s">
+        <v>71</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>19</v>
@@ -2130,10 +2130,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="45"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>20</v>
@@ -2146,10 +2146,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="47" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="19" t="s">
@@ -2166,8 +2166,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="48"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="48"/>
       <c r="C9" s="19" t="s">
         <v>50</v>
       </c>
@@ -2202,14 +2202,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="49" t="s">
-        <v>74</v>
+      <c r="B11" s="47" t="s">
+        <v>72</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>52</v>
@@ -2222,10 +2222,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="50"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>53</v>
@@ -2238,10 +2238,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="47" t="s">
         <v>54</v>
       </c>
       <c r="C13" s="19" t="s">
@@ -2258,10 +2258,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
-      <c r="B14" s="52"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>53</v>
@@ -2274,8 +2274,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
-      <c r="B15" s="50"/>
+      <c r="A15" s="46"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="19" t="s">
         <v>56</v>
       </c>
@@ -2290,14 +2290,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="51" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>58</v>
+        <v>124</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>52</v>
@@ -2310,10 +2310,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
-      <c r="B17" s="45"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="19" t="s">
-        <v>59</v>
+        <v>125</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>53</v>
@@ -2330,10 +2330,10 @@
         <v>31</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>53</v>
@@ -2346,82 +2346,82 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="49"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="49"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="46"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="24" t="s">
+      <c r="E22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="19" t="s">
+      <c r="C23" s="20" t="s">
         <v>79</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>81</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>52</v>
@@ -2434,10 +2434,10 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
-      <c r="B24" s="50"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="48"/>
       <c r="C24" s="20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D24" s="24" t="s">
         <v>53</v>
@@ -2474,49 +2474,49 @@
         <v>35</v>
       </c>
       <c r="B26" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C27" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D27" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="52"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="25" t="s">
         <v>70</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="46"/>
-      <c r="B28" s="45"/>
-      <c r="C28" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>72</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>5</v>
@@ -2530,49 +2530,49 @@
         <v>36</v>
       </c>
       <c r="B29" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C30" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="45" t="s">
+      <c r="D30" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="46"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="25" t="s">
         <v>85</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
-      <c r="B31" s="45"/>
-      <c r="C31" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>87</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>5</v>
@@ -2586,13 +2586,13 @@
         <v>38</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>5</v>
@@ -2606,49 +2606,49 @@
         <v>39</v>
       </c>
       <c r="B33" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" s="29" t="s">
+      <c r="E34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="46"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="30" t="s">
         <v>93</v>
-      </c>
-      <c r="D34" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="48"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="D35" s="30" t="s">
-        <v>95</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>5</v>
@@ -2662,10 +2662,10 @@
         <v>41</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D36" s="24" t="s">
         <v>53</v>
@@ -2682,13 +2682,13 @@
         <v>42</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>5</v>
@@ -2722,13 +2722,13 @@
         <v>44</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>5</v>
@@ -2742,13 +2742,13 @@
         <v>45</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>5</v>
@@ -2779,16 +2779,16 @@
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B42" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="43" t="s">
         <v>115</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="D42" s="43" t="s">
-        <v>117</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>5</v>
@@ -2799,13 +2799,13 @@
     </row>
     <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B43" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" s="19" t="s">
         <v>118</v>
-      </c>
-      <c r="B43" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>120</v>
       </c>
       <c r="D43" s="24" t="s">
         <v>53</v>
@@ -2819,13 +2819,13 @@
     </row>
     <row r="44" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="26" t="s">
         <v>104</v>
-      </c>
-      <c r="B44" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>106</v>
       </c>
       <c r="D44" s="27"/>
       <c r="E44" s="5" t="s">
@@ -2838,18 +2838,6 @@
   </sheetData>
   <autoFilter ref="A1:E27"/>
   <mergeCells count="20">
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A27:A28"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A16:A17"/>
@@ -2858,6 +2846,18 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E24 E29:E1048576">
     <cfRule type="cellIs" dxfId="7" priority="31" operator="equal">

</xml_diff>

<commit_message>
-	Prise en compte de la surchage de la définition d’un bloc de donnée via le Resize block, -	Prise en compte d’un nouveau paramètre NvMSingleBlockCallback
</commit_message>
<xml_diff>
--- a/MEM_configurator_test_plan.xlsx
+++ b/MEM_configurator_test_plan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristi\PycharmProjects\MEM_Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcsterpu\PycharmProjects\MEM_Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212FE071-6213-41FE-BA8D-16338E67AD90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000" activeTab="1"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="3" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="140">
   <si>
     <t>Requirements</t>
   </si>
@@ -988,12 +989,115 @@
       </rPr>
       <t>: Provide to the tool on block that references three ports, and another file which does not contain the interfaces referenced by these ports</t>
     </r>
+  </si>
+  <si>
+    <t>TRS.MEMCFG.GEN.015</t>
+  </si>
+  <si>
+    <t>- Check that the output file contains the values found in the overloaded block</t>
+  </si>
+  <si>
+    <t>Take into account the overriding parameters</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Provide to the tool the definition of an existing block with the same name in the correct input parameter</t>
+    </r>
+  </si>
+  <si>
+    <t>TRS.MEMCFG.CHECK.013</t>
+  </si>
+  <si>
+    <t>Check that the CALLBACK function name is safely taken into account</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Provide to the tool the definition of a block definition which has two different callback functions present</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Provide to the tool the definition of a block definition which has only one callback function</t>
+    </r>
+  </si>
+  <si>
+    <t>- Check that the tool does not produce the output file
+- Check that the tool will generate an error in the log</t>
+  </si>
+  <si>
+    <t>- Check that the tool will produce an output file with the correct value of the callback function</t>
+  </si>
+  <si>
+    <t>TRS.MEMCFG.GEN.018</t>
+  </si>
+  <si>
+    <t>Take into account the "SINGLE-BLOCK-CALL-BACK-FUNCTION" parameter given in the configuration file</t>
+  </si>
+  <si>
+    <t>Test 1: Provide to the tool the definion of a block which has the "SINGLE-BLOCK-CALL-BACK-FUNCTION" parameter set in the configuration file</t>
+  </si>
+  <si>
+    <t>- Check in the output NvM file that the parameter is set with the precised value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1348,7 +1452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1460,6 +1564,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1478,11 +1588,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1844,21 +1963,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="68.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="8" customWidth="1"/>
+    <col min="1" max="2" width="9.1328125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="68.3984375" customWidth="1"/>
+    <col min="4" max="4" width="9.1328125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -1872,7 +1991,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
@@ -1886,97 +2005,97 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="16"/>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10"/>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
       <c r="D16" s="9"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
       <c r="D17" s="9"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
@@ -1989,27 +2108,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="79.140625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.3984375" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.86328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="79.1328125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="46.265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.265625" style="2" customWidth="1"/>
     <col min="6" max="6" width="10" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -2029,7 +2148,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="28.9" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A2" s="32" t="s">
         <v>21</v>
       </c>
@@ -2049,7 +2168,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="32" t="s">
         <v>22</v>
       </c>
@@ -2069,7 +2188,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="32" t="s">
         <v>23</v>
       </c>
@@ -2089,7 +2208,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="33" t="s">
         <v>24</v>
       </c>
@@ -2109,11 +2228,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="52" t="s">
+    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="45" t="s">
         <v>71</v>
       </c>
       <c r="C6" s="19" t="s">
@@ -2129,9 +2248,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="51"/>
+    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="46"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="19" t="s">
         <v>120</v>
       </c>
@@ -2145,11 +2264,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+    <row r="8" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A8" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="49" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="19" t="s">
@@ -2165,9 +2284,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="48"/>
+    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="48"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="19" t="s">
         <v>50</v>
       </c>
@@ -2181,7 +2300,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="32" t="s">
         <v>27</v>
       </c>
@@ -2201,11 +2320,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="49" t="s">
         <v>72</v>
       </c>
       <c r="C11" s="19" t="s">
@@ -2221,9 +2340,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="48"/>
+    <row r="12" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="48"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="19" t="s">
         <v>122</v>
       </c>
@@ -2237,11 +2356,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+    <row r="13" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="49" t="s">
         <v>54</v>
       </c>
       <c r="C13" s="19" t="s">
@@ -2257,9 +2376,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="50"/>
+    <row r="14" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="51"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="19" t="s">
         <v>74</v>
       </c>
@@ -2273,9 +2392,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="48"/>
+    <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="48"/>
+      <c r="B15" s="50"/>
       <c r="C15" s="19" t="s">
         <v>56</v>
       </c>
@@ -2289,11 +2408,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
+    <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="45" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="19" t="s">
@@ -2309,9 +2428,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
-      <c r="B17" s="51"/>
+    <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="46"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="19" t="s">
         <v>125</v>
       </c>
@@ -2325,7 +2444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="32" t="s">
         <v>31</v>
       </c>
@@ -2345,11 +2464,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
+    <row r="19" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="49" t="s">
         <v>60</v>
       </c>
       <c r="C19" s="19" t="s">
@@ -2365,9 +2484,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="50"/>
+    <row r="20" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="51"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="19" t="s">
         <v>76</v>
       </c>
@@ -2381,9 +2500,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="50"/>
+    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="51"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="19" t="s">
         <v>77</v>
       </c>
@@ -2397,9 +2516,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
-      <c r="B22" s="48"/>
+    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="48"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="19" t="s">
         <v>78</v>
       </c>
@@ -2413,11 +2532,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
+    <row r="23" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="49" t="s">
         <v>63</v>
       </c>
       <c r="C23" s="20" t="s">
@@ -2433,9 +2552,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
-      <c r="B24" s="48"/>
+    <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="48"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="20" t="s">
         <v>80</v>
       </c>
@@ -2449,7 +2568,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="32" t="s">
         <v>34</v>
       </c>
@@ -2469,7 +2588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="32" t="s">
         <v>35</v>
       </c>
@@ -2489,11 +2608,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="52" t="s">
+    <row r="27" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="45" t="s">
         <v>66</v>
       </c>
       <c r="C27" s="19" t="s">
@@ -2509,9 +2628,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
-      <c r="B28" s="51"/>
+    <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="46"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="19" t="s">
         <v>82</v>
       </c>
@@ -2525,7 +2644,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A29" s="32" t="s">
         <v>36</v>
       </c>
@@ -2545,11 +2664,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="45" t="s">
+    <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A30" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="51" t="s">
+      <c r="B30" s="45" t="s">
         <v>83</v>
       </c>
       <c r="C30" s="19" t="s">
@@ -2565,9 +2684,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="46"/>
-      <c r="B31" s="51"/>
+    <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A31" s="48"/>
+      <c r="B31" s="45"/>
       <c r="C31" s="19" t="s">
         <v>82</v>
       </c>
@@ -2581,7 +2700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32" s="34" t="s">
         <v>38</v>
       </c>
@@ -2601,7 +2720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" s="34" t="s">
         <v>39</v>
       </c>
@@ -2621,11 +2740,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="45" t="s">
+    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="49" t="s">
         <v>89</v>
       </c>
       <c r="C34" s="29" t="s">
@@ -2641,9 +2760,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="46"/>
-      <c r="B35" s="48"/>
+    <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A35" s="48"/>
+      <c r="B35" s="50"/>
       <c r="C35" s="29" t="s">
         <v>92</v>
       </c>
@@ -2657,7 +2776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A36" s="34" t="s">
         <v>41</v>
       </c>
@@ -2677,7 +2796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A37" s="34" t="s">
         <v>42</v>
       </c>
@@ -2697,7 +2816,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="41" t="s">
         <v>43</v>
       </c>
@@ -2717,7 +2836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="34" t="s">
         <v>44</v>
       </c>
@@ -2737,7 +2856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="34" t="s">
         <v>45</v>
       </c>
@@ -2757,7 +2876,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="41" t="s">
         <v>46</v>
       </c>
@@ -2777,67 +2896,151 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A42" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A43" s="53" t="s">
+        <v>130</v>
+      </c>
+      <c r="B43" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A44" s="54"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="D44" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A45" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="D45" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A46" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B42" s="42" t="s">
+      <c r="B46" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="C42" s="29" t="s">
+      <c r="C46" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="D42" s="43" t="s">
+      <c r="D46" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="E42" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="41" t="s">
+      <c r="E46" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A47" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="B43" s="42" t="s">
+      <c r="B47" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C47" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="24" t="s">
+      <c r="D47" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E43" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="35" t="s">
+      <c r="E47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A48" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="B44" s="40" t="s">
+      <c r="B48" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="C44" s="26" t="s">
+      <c r="C48" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="D44" s="27"/>
-      <c r="E44" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F44" s="6" t="s">
+      <c r="D48" s="27"/>
+      <c r="E48" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" s="6" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E27"/>
-  <mergeCells count="20">
+  <autoFilter ref="A1:E27" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <mergeCells count="22">
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A16:A17"/>
@@ -2852,12 +3055,6 @@
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E24 E29:E1048576">
     <cfRule type="cellIs" dxfId="7" priority="31" operator="equal">
@@ -2867,12 +3064,12 @@
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F24 F29:F44">
+  <conditionalFormatting sqref="F2:F24 F29:F48">
     <cfRule type="cellIs" dxfId="5" priority="30" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F24 F29:F44">
+  <conditionalFormatting sqref="F2:F24 F29:F48">
     <cfRule type="cellIs" dxfId="4" priority="29" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
@@ -2896,10 +3093,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E44">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E48" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"done, not done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F44">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F48" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"YES, NO"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
FELP 84849 :       [TOOLS 2020.06] : Addition of the feature of the block writting during a WriteAll
</commit_message>
<xml_diff>
--- a/MEM_configurator_test_plan.xlsx
+++ b/MEM_configurator_test_plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcsterpu\PycharmProjects\MEM_Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212FE071-6213-41FE-BA8D-16338E67AD90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7400C021-3C9B-4668-8AF4-EE9D38ACC240}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1564,44 +1564,44 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2112,7 +2112,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
@@ -2229,10 +2229,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="56" t="s">
         <v>71</v>
       </c>
       <c r="C6" s="19" t="s">
@@ -2249,8 +2249,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="46"/>
-      <c r="B7" s="45"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="19" t="s">
         <v>120</v>
       </c>
@@ -2265,10 +2265,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="48" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="19" t="s">
@@ -2285,8 +2285,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="48"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="19" t="s">
         <v>50</v>
       </c>
@@ -2321,10 +2321,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="48" t="s">
         <v>72</v>
       </c>
       <c r="C11" s="19" t="s">
@@ -2341,8 +2341,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="48"/>
-      <c r="B12" s="50"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="19" t="s">
         <v>122</v>
       </c>
@@ -2357,10 +2357,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="48" t="s">
         <v>54</v>
       </c>
       <c r="C13" s="19" t="s">
@@ -2377,8 +2377,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="51"/>
-      <c r="B14" s="52"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="19" t="s">
         <v>74</v>
       </c>
@@ -2393,8 +2393,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="48"/>
-      <c r="B15" s="50"/>
+      <c r="A15" s="47"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="19" t="s">
         <v>56</v>
       </c>
@@ -2409,10 +2409,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="56" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="19" t="s">
@@ -2429,8 +2429,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A17" s="46"/>
-      <c r="B17" s="45"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="19" t="s">
         <v>125</v>
       </c>
@@ -2465,10 +2465,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="48" t="s">
         <v>60</v>
       </c>
       <c r="C19" s="19" t="s">
@@ -2485,8 +2485,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="51"/>
-      <c r="B20" s="52"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="19" t="s">
         <v>76</v>
       </c>
@@ -2501,8 +2501,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="51"/>
-      <c r="B21" s="52"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="51"/>
       <c r="C21" s="19" t="s">
         <v>77</v>
       </c>
@@ -2517,8 +2517,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="48"/>
-      <c r="B22" s="50"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="49"/>
       <c r="C22" s="19" t="s">
         <v>78</v>
       </c>
@@ -2533,10 +2533,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="48" t="s">
         <v>63</v>
       </c>
       <c r="C23" s="20" t="s">
@@ -2553,8 +2553,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A24" s="48"/>
-      <c r="B24" s="50"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="20" t="s">
         <v>80</v>
       </c>
@@ -2609,10 +2609,10 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="56" t="s">
         <v>66</v>
       </c>
       <c r="C27" s="19" t="s">
@@ -2629,8 +2629,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="46"/>
-      <c r="B28" s="45"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="56"/>
       <c r="C28" s="19" t="s">
         <v>82</v>
       </c>
@@ -2665,10 +2665,10 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="45" t="s">
+      <c r="B30" s="56" t="s">
         <v>83</v>
       </c>
       <c r="C30" s="19" t="s">
@@ -2685,8 +2685,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A31" s="48"/>
-      <c r="B31" s="45"/>
+      <c r="A31" s="47"/>
+      <c r="B31" s="56"/>
       <c r="C31" s="19" t="s">
         <v>82</v>
       </c>
@@ -2741,10 +2741,10 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="47" t="s">
+      <c r="A34" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="48" t="s">
         <v>89</v>
       </c>
       <c r="C34" s="29" t="s">
@@ -2761,8 +2761,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A35" s="48"/>
-      <c r="B35" s="50"/>
+      <c r="A35" s="47"/>
+      <c r="B35" s="49"/>
       <c r="C35" s="29" t="s">
         <v>92</v>
       </c>
@@ -2917,10 +2917,10 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A43" s="53" t="s">
+      <c r="A43" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="B43" s="55" t="s">
+      <c r="B43" s="54" t="s">
         <v>131</v>
       </c>
       <c r="C43" s="44" t="s">
@@ -2937,8 +2937,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A44" s="54"/>
-      <c r="B44" s="56"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="55"/>
       <c r="C44" s="44" t="s">
         <v>133</v>
       </c>
@@ -2956,7 +2956,7 @@
       <c r="A45" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="B45" s="57" t="s">
+      <c r="B45" s="45" t="s">
         <v>137</v>
       </c>
       <c r="C45" s="44" t="s">
@@ -3033,12 +3033,6 @@
   </sheetData>
   <autoFilter ref="A1:E27" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="22">
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="B6:B7"/>
@@ -3055,6 +3049,12 @@
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E24 E29:E1048576">
     <cfRule type="cellIs" dxfId="7" priority="31" operator="equal">

</xml_diff>